<commit_message>
finish up the else draft
</commit_message>
<xml_diff>
--- a/id_output/missing_id_list.xlsx
+++ b/id_output/missing_id_list.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">first</t>
   </si>
@@ -42,15 +42,6 @@
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alejandro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vásquez Echeverría</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimating the reproducibility of psychological science</t>
   </si>
 </sst>
 </file>
@@ -430,20 +421,6 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>